<commit_message>
Added LIMIT and OFFSET
</commit_message>
<xml_diff>
--- a/AppDefinition.xlsx
+++ b/AppDefinition.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\workspace\xltemplating\AppGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\AppGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="14" r:id="rId1"/>
@@ -898,10 +898,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ddl_mysql.txt</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>entity.txt</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1226,6 +1222,10 @@
   </si>
   <si>
     <t>URL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ddl_h2.txt</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1674,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1718,7 +1718,7 @@
         <v>231</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G1" t="s">
         <v>193</v>
@@ -1739,30 +1739,30 @@
         <v>196</v>
       </c>
       <c r="P1" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="Q1" s="14" t="s">
-        <v>261</v>
-      </c>
       <c r="S1" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="T1" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="T1" s="9" t="s">
-        <v>302</v>
-      </c>
       <c r="W1" s="18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="X1" t="s">
+        <v>306</v>
+      </c>
+      <c r="Y1" t="s">
         <v>307</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="V2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1770,7 +1770,7 @@
         <v>183</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -1798,7 +1798,7 @@
         <v>197</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C5" t="s">
         <v>81</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s">
         <v>111</v>
@@ -1915,7 +1915,7 @@
         <v>CartMapperGen</v>
       </c>
       <c r="V6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="W6" s="18" t="str">
         <f t="shared" ref="W6:W11" si="11">"/"&amp;LOWER(B6)&amp;V6</f>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C7" t="s">
         <v>55</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C8" t="s">
         <v>100</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C9" t="s">
         <v>106</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C10" t="s">
         <v>108</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C11" t="s">
         <v>144</v>
@@ -2347,46 +2347,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>257</v>
-      </c>
       <c r="I1" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>288</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2407,7 +2407,7 @@
     </row>
     <row r="5" spans="1:16" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="21"/>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="8" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>207</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="9" t="b">
         <f>LEN(G9)&gt;5</f>
@@ -2460,7 +2460,7 @@
         <v>212</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F9" s="9" t="str">
         <f>"./generated/"&amp;Entities!G5&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S5,".","/")</f>
@@ -2471,14 +2471,14 @@
         <v>CustomerMapperGen.java</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J9" s="9" t="str">
         <f>"entities["&amp;C9&amp;"]"</f>
         <v>entities[0]</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L9" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C5&amp;"'])"</f>
@@ -2502,7 +2502,7 @@
         <v>212</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F10" s="10" t="str">
         <f>"./generated/"&amp;Entities!G6&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S6,".","/")</f>
@@ -2513,14 +2513,14 @@
         <v>CartMapperGen.java</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J10" s="9" t="str">
         <f t="shared" ref="J10:J19" si="1">"entities["&amp;C10&amp;"]"</f>
         <v>entities[1]</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L10" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C6&amp;"'])"</f>
@@ -2540,7 +2540,7 @@
         <v>212</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F11" s="10" t="str">
         <f>"./generated/"&amp;Entities!G7&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S7,".","/")</f>
@@ -2551,14 +2551,14 @@
         <v>OrderMapperGen.java</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J11" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[2]</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L11" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C7&amp;"'])"</f>
@@ -2578,7 +2578,7 @@
         <v>212</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F12" s="10" t="str">
         <f>"./generated/"&amp;Entities!G8&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S8,".","/")</f>
@@ -2589,14 +2589,14 @@
         <v>OrderDetailMapperGen.java</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J12" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[3]</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L12" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C8&amp;"'])"</f>
@@ -2616,7 +2616,7 @@
         <v>212</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F13" s="10" t="str">
         <f>"./generated/"&amp;Entities!G9&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S9,".","/")</f>
@@ -2627,14 +2627,14 @@
         <v>ProductMapperGen.java</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J13" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[4]</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L13" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C9&amp;"'])"</f>
@@ -2654,7 +2654,7 @@
         <v>212</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F14" s="10" t="str">
         <f>"./generated/"&amp;Entities!G10&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S10,".","/")</f>
@@ -2665,14 +2665,14 @@
         <v>StockMapperGen.java</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J14" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[5]</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L14" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C10&amp;"'])"</f>
@@ -2692,7 +2692,7 @@
         <v>212</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F15" s="10" t="str">
         <f>"./generated/"&amp;Entities!G11&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S11,".","/")</f>
@@ -2703,14 +2703,14 @@
         <v>AddressMasterMapperGen.java</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J15" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[6]</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L15" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C11&amp;"'])"</f>
@@ -2730,7 +2730,7 @@
         <v>212</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F16" s="10" t="str">
         <f>"./generated/"&amp;Entities!G12&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S12,".","/")</f>
@@ -2741,14 +2741,14 @@
         <v>.java</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J16" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[7]</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L16" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C12&amp;"'])"</f>
@@ -2768,7 +2768,7 @@
         <v>212</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F17" s="10" t="str">
         <f>"./generated/"&amp;Entities!G13&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S13,".","/")</f>
@@ -2779,14 +2779,14 @@
         <v>.java</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J17" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[8]</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L17" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C13&amp;"'])"</f>
@@ -2806,7 +2806,7 @@
         <v>212</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F18" s="10" t="str">
         <f>"./generated/"&amp;Entities!G14&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S14,".","/")</f>
@@ -2817,14 +2817,14 @@
         <v>.java</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J18" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[9]</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L18" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C14&amp;"'])"</f>
@@ -2844,7 +2844,7 @@
         <v>212</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F19" s="10" t="str">
         <f>"./generated/"&amp;Entities!G15&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!S15,".","/")</f>
@@ -2855,14 +2855,14 @@
         <v>.java</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J19" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[10]</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L19" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C15&amp;"'])"</f>
@@ -2912,46 +2912,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>257</v>
-      </c>
       <c r="I1" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J1" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>288</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2972,7 +2972,7 @@
     </row>
     <row r="5" spans="1:16" ht="121.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="21"/>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="8" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>207</v>
@@ -3012,7 +3012,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="9" t="b">
         <f>LEN(G9)&gt;5</f>
@@ -3025,7 +3025,7 @@
         <v>212</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F9" s="9" t="str">
         <f>"./generated/"&amp;Entities!G5&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S5,".","/")</f>
@@ -3036,14 +3036,14 @@
         <v>CustomerMapperGen.xml</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J9" s="9" t="str">
         <f>"entities["&amp;C9&amp;"]"</f>
         <v>entities[0]</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L9" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C5&amp;"'])"</f>
@@ -3067,7 +3067,7 @@
         <v>212</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F10" s="9" t="str">
         <f>"./generated/"&amp;Entities!G6&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S6,".","/")</f>
@@ -3078,14 +3078,14 @@
         <v>CartMapperGen.xml</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J10" s="9" t="str">
         <f t="shared" ref="J10:J19" si="1">"entities["&amp;C10&amp;"]"</f>
         <v>entities[1]</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L10" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C6&amp;"'])"</f>
@@ -3105,7 +3105,7 @@
         <v>212</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F11" s="9" t="str">
         <f>"./generated/"&amp;Entities!G7&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S7,".","/")</f>
@@ -3116,14 +3116,14 @@
         <v>OrderMapperGen.xml</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J11" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[2]</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L11" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C7&amp;"'])"</f>
@@ -3143,7 +3143,7 @@
         <v>212</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F12" s="9" t="str">
         <f>"./generated/"&amp;Entities!G8&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S8,".","/")</f>
@@ -3154,14 +3154,14 @@
         <v>OrderDetailMapperGen.xml</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J12" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[3]</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L12" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C8&amp;"'])"</f>
@@ -3181,7 +3181,7 @@
         <v>212</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F13" s="9" t="str">
         <f>"./generated/"&amp;Entities!G9&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S9,".","/")</f>
@@ -3192,14 +3192,14 @@
         <v>ProductMapperGen.xml</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J13" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[4]</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L13" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C9&amp;"'])"</f>
@@ -3219,7 +3219,7 @@
         <v>212</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F14" s="9" t="str">
         <f>"./generated/"&amp;Entities!G10&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S10,".","/")</f>
@@ -3230,14 +3230,14 @@
         <v>StockMapperGen.xml</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J14" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[5]</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L14" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C10&amp;"'])"</f>
@@ -3257,7 +3257,7 @@
         <v>212</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F15" s="9" t="str">
         <f>"./generated/"&amp;Entities!G11&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S11,".","/")</f>
@@ -3268,14 +3268,14 @@
         <v>AddressMasterMapperGen.xml</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J15" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[6]</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L15" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C11&amp;"'])"</f>
@@ -3295,7 +3295,7 @@
         <v>212</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F16" s="9" t="str">
         <f>"./generated/"&amp;Entities!G12&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S12,".","/")</f>
@@ -3306,14 +3306,14 @@
         <v>.xml</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J16" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[7]</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L16" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C12&amp;"'])"</f>
@@ -3333,7 +3333,7 @@
         <v>212</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F17" s="9" t="str">
         <f>"./generated/"&amp;Entities!G13&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S13,".","/")</f>
@@ -3344,14 +3344,14 @@
         <v>.xml</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J17" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[8]</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L17" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C13&amp;"'])"</f>
@@ -3371,7 +3371,7 @@
         <v>212</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F18" s="9" t="str">
         <f>"./generated/"&amp;Entities!G14&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S14,".","/")</f>
@@ -3382,14 +3382,14 @@
         <v>.xml</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J18" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[9]</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L18" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C14&amp;"'])"</f>
@@ -3409,7 +3409,7 @@
         <v>212</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F19" s="9" t="str">
         <f>"./generated/"&amp;Entities!G15&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!S15,".","/")</f>
@@ -3420,14 +3420,14 @@
         <v>.xml</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J19" s="9" t="str">
         <f t="shared" si="1"/>
         <v>entities[10]</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L19" s="9" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C15&amp;"'])"</f>
@@ -5362,7 +5362,7 @@
         <v>216</v>
       </c>
       <c r="E1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F1" t="s">
         <v>143</v>
@@ -5663,7 +5663,7 @@
         <v>133</v>
       </c>
       <c r="H7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5907,16 +5907,16 @@
         <v>82</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>246</v>
       </c>
       <c r="K12" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6116,7 +6116,7 @@
         <v>112</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>129</v>
@@ -6319,7 +6319,7 @@
         <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F20" t="s">
         <v>121</v>
@@ -6983,10 +6983,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C1" t="s">
         <v>148</v>
@@ -7008,10 +7008,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" t="s">
         <v>136</v>
@@ -7022,7 +7022,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
         <v>137</v>
@@ -7033,24 +7033,24 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" t="s">
         <v>246</v>
       </c>
-      <c r="C5" t="s">
-        <v>247</v>
-      </c>
       <c r="D5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -7081,92 +7081,92 @@
   <sheetData>
     <row r="1" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>277</v>
-      </c>
       <c r="L1" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>292</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H2" t="s">
         <v>294</v>
       </c>
-      <c r="G2" t="s">
-        <v>264</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>298</v>
-      </c>
       <c r="L2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H3" t="s">
         <v>95</v>
       </c>
       <c r="L3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -7174,16 +7174,16 @@
         <v>82</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G4" t="s">
         <v>112</v>
       </c>
       <c r="H4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -7196,8 +7196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -7224,46 +7224,46 @@
         <v>215</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" t="s">
         <v>252</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>253</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>254</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>255</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>256</v>
       </c>
-      <c r="G1" t="s">
-        <v>257</v>
-      </c>
       <c r="I1" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>288</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -7284,10 +7284,10 @@
     </row>
     <row r="5" spans="1:16" ht="312.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -7306,7 +7306,7 @@
     </row>
     <row r="8" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" t="s">
         <v>207</v>
@@ -7326,7 +7326,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="4" t="b">
         <v>1</v>
@@ -7338,14 +7338,14 @@
         <v>212</v>
       </c>
       <c r="E9" t="s">
-        <v>233</v>
+        <v>316</v>
       </c>
       <c r="F9" s="17" t="str">
         <f>"./generated/"&amp;Entities!G5&amp;"/src/main/resources/"</f>
         <v>./generated/webshop/src/main/resources/</v>
       </c>
       <c r="G9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -7362,7 +7362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -7391,46 +7391,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>257</v>
-      </c>
       <c r="I1" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>288</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -7451,7 +7451,7 @@
     </row>
     <row r="5" spans="1:16" ht="218.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -7471,7 +7471,7 @@
     </row>
     <row r="8" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>207</v>
@@ -7491,7 +7491,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="16" t="b">
         <f>LEN(G9)&gt;5</f>
@@ -7504,7 +7504,7 @@
         <v>212</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F9" s="16" t="str">
         <f>"./generated/"&amp;Entities!G5&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X5,".","/")</f>
@@ -7515,14 +7515,14 @@
         <v>CustomerApi.java</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J9" s="16" t="str">
         <f>"entities["&amp;C9&amp;"]"</f>
         <v>entities[0]</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L9" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C5&amp;"'])"</f>
@@ -7546,7 +7546,7 @@
         <v>212</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F10" s="16" t="str">
         <f>"./generated/"&amp;Entities!G6&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X6,".","/")</f>
@@ -7557,14 +7557,14 @@
         <v>CartApi.java</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J10" s="16" t="str">
         <f t="shared" ref="J10:J19" si="1">"entities["&amp;C10&amp;"]"</f>
         <v>entities[1]</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L10" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C6&amp;"'])"</f>
@@ -7584,7 +7584,7 @@
         <v>212</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F11" s="16" t="str">
         <f>"./generated/"&amp;Entities!G7&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X7,".","/")</f>
@@ -7595,14 +7595,14 @@
         <v>OrderApi.java</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J11" s="16" t="str">
         <f t="shared" si="1"/>
         <v>entities[2]</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L11" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C7&amp;"'])"</f>
@@ -7622,7 +7622,7 @@
         <v>212</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F12" s="16" t="str">
         <f>"./generated/"&amp;Entities!G8&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X8,".","/")</f>
@@ -7633,14 +7633,14 @@
         <v>OrderDetailApi.java</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J12" s="16" t="str">
         <f t="shared" si="1"/>
         <v>entities[3]</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L12" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C8&amp;"'])"</f>
@@ -7660,7 +7660,7 @@
         <v>212</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F13" s="16" t="str">
         <f>"./generated/"&amp;Entities!G9&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X9,".","/")</f>
@@ -7671,14 +7671,14 @@
         <v>ProductApi.java</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J13" s="16" t="str">
         <f t="shared" si="1"/>
         <v>entities[4]</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L13" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C9&amp;"'])"</f>
@@ -7698,7 +7698,7 @@
         <v>212</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F14" s="16" t="str">
         <f>"./generated/"&amp;Entities!G10&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X10,".","/")</f>
@@ -7709,14 +7709,14 @@
         <v>StockApi.java</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J14" s="16" t="str">
         <f t="shared" si="1"/>
         <v>entities[5]</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L14" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C10&amp;"'])"</f>
@@ -7736,7 +7736,7 @@
         <v>212</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F15" s="16" t="str">
         <f>"./generated/"&amp;Entities!G11&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X11,".","/")</f>
@@ -7747,14 +7747,14 @@
         <v>AddressMasterApi.java</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J15" s="16" t="str">
         <f t="shared" si="1"/>
         <v>entities[6]</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L15" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C11&amp;"'])"</f>
@@ -7774,7 +7774,7 @@
         <v>212</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F16" s="16" t="str">
         <f>"./generated/"&amp;Entities!G12&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X12,".","/")</f>
@@ -7785,14 +7785,14 @@
         <v>.java</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J16" s="16" t="str">
         <f t="shared" si="1"/>
         <v>entities[7]</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L16" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C12&amp;"'])"</f>
@@ -7812,7 +7812,7 @@
         <v>212</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F17" s="16" t="str">
         <f>"./generated/"&amp;Entities!G13&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X13,".","/")</f>
@@ -7823,14 +7823,14 @@
         <v>.java</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J17" s="16" t="str">
         <f t="shared" si="1"/>
         <v>entities[8]</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L17" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C13&amp;"'])"</f>
@@ -7850,7 +7850,7 @@
         <v>212</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F18" s="16" t="str">
         <f>"./generated/"&amp;Entities!G14&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X14,".","/")</f>
@@ -7861,14 +7861,14 @@
         <v>.java</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J18" s="16" t="str">
         <f t="shared" si="1"/>
         <v>entities[9]</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L18" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C14&amp;"'])"</f>
@@ -7888,7 +7888,7 @@
         <v>212</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F19" s="16" t="str">
         <f>"./generated/"&amp;Entities!G15&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!X15,".","/")</f>
@@ -7899,14 +7899,14 @@
         <v>.java</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J19" s="16" t="str">
         <f t="shared" si="1"/>
         <v>entities[10]</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L19" s="16" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C15&amp;"'])"</f>
@@ -7956,46 +7956,46 @@
         <v>215</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>257</v>
-      </c>
       <c r="I1" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>288</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -8016,7 +8016,7 @@
     </row>
     <row r="5" spans="1:16" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="21"/>
@@ -8036,7 +8036,7 @@
     </row>
     <row r="8" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>207</v>
@@ -8056,7 +8056,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="4" t="b">
         <f>LEN(G9)&gt;5</f>
@@ -8069,7 +8069,7 @@
         <v>212</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F9" s="4" t="str">
         <f>"./generated/"&amp;Entities!G5&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J5,".","/")</f>
@@ -8080,14 +8080,14 @@
         <v>Customer.java</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J9" s="4" t="str">
         <f>"entities["&amp;C9&amp;"]"</f>
         <v>entities[0]</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L9" s="4" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C5&amp;"'])"</f>
@@ -8111,7 +8111,7 @@
         <v>212</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F10" s="9" t="str">
         <f>"./generated/"&amp;Entities!G6&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J6,".","/")</f>
@@ -8122,14 +8122,14 @@
         <v>Cart.java</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J10" s="4" t="str">
         <f t="shared" ref="J10:J15" si="1">"entities["&amp;C10&amp;"]"</f>
         <v>entities[1]</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L10" s="4" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C6&amp;"'])"</f>
@@ -8149,7 +8149,7 @@
         <v>212</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F11" s="9" t="str">
         <f>"./generated/"&amp;Entities!G7&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J7,".","/")</f>
@@ -8160,14 +8160,14 @@
         <v>Order.java</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>entities[2]</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L11" s="4" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C7&amp;"'])"</f>
@@ -8187,7 +8187,7 @@
         <v>212</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F12" s="9" t="str">
         <f>"./generated/"&amp;Entities!G8&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J8,".","/")</f>
@@ -8198,14 +8198,14 @@
         <v>OrderDetail.java</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>entities[3]</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L12" s="4" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C8&amp;"'])"</f>
@@ -8225,7 +8225,7 @@
         <v>212</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F13" s="9" t="str">
         <f>"./generated/"&amp;Entities!G9&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J9,".","/")</f>
@@ -8236,14 +8236,14 @@
         <v>Product.java</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>entities[4]</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L13" s="4" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C9&amp;"'])"</f>
@@ -8263,7 +8263,7 @@
         <v>212</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F14" s="9" t="str">
         <f>"./generated/"&amp;Entities!G10&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J10,".","/")</f>
@@ -8274,14 +8274,14 @@
         <v>Stock.java</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J14" s="4" t="str">
         <f t="shared" si="1"/>
         <v>entities[5]</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L14" s="4" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C10&amp;"'])"</f>
@@ -8301,7 +8301,7 @@
         <v>212</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F15" s="9" t="str">
         <f>"./generated/"&amp;Entities!G11&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J11,".","/")</f>
@@ -8312,14 +8312,14 @@
         <v>AddressMaster.java</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>entities[6]</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L15" s="4" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C11&amp;"'])"</f>
@@ -8339,7 +8339,7 @@
         <v>212</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F16" s="9" t="str">
         <f>"./generated/"&amp;Entities!G12&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J12,".","/")</f>
@@ -8350,14 +8350,14 @@
         <v>.java</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" ref="J16:J19" si="3">"entities["&amp;C16&amp;"]"</f>
         <v>entities[7]</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L16" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C12&amp;"'])"</f>
@@ -8378,7 +8378,7 @@
         <v>212</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F17" s="9" t="str">
         <f>"./generated/"&amp;Entities!G13&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J13,".","/")</f>
@@ -8389,14 +8389,14 @@
         <v>.java</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J17" s="6" t="str">
         <f t="shared" si="3"/>
         <v>entities[8]</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L17" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C13&amp;"'])"</f>
@@ -8417,7 +8417,7 @@
         <v>212</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F18" s="9" t="str">
         <f>"./generated/"&amp;Entities!G14&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J14,".","/")</f>
@@ -8428,14 +8428,14 @@
         <v>.java</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J18" s="6" t="str">
         <f t="shared" si="3"/>
         <v>entities[9]</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L18" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C14&amp;"'])"</f>
@@ -8456,7 +8456,7 @@
         <v>212</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F19" s="9" t="str">
         <f>"./generated/"&amp;Entities!G15&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!J15,".","/")</f>
@@ -8467,14 +8467,14 @@
         <v>.java</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J19" s="6" t="str">
         <f t="shared" si="3"/>
         <v>entities[10]</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L19" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C15&amp;"'])"</f>
@@ -8525,46 +8525,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>257</v>
-      </c>
       <c r="I1" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>288</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -8585,7 +8585,7 @@
     </row>
     <row r="5" spans="1:16" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="21"/>
@@ -8605,7 +8605,7 @@
     </row>
     <row r="8" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>207</v>
@@ -8625,7 +8625,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="6" t="b">
         <f>LEN(G9)&gt;5</f>
@@ -8638,7 +8638,7 @@
         <v>212</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F9" s="6" t="str">
         <f>"./generated/"&amp;Entities!G5&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M5,".","/")</f>
@@ -8649,14 +8649,14 @@
         <v>CustomerDao.java</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J9" s="6" t="str">
         <f>"entities["&amp;C9&amp;"]"</f>
         <v>entities[0]</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L9" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C5&amp;"'])"</f>
@@ -8680,7 +8680,7 @@
         <v>212</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F10" s="9" t="str">
         <f>"./generated/"&amp;Entities!G6&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M6,".","/")</f>
@@ -8691,14 +8691,14 @@
         <v>CartDao.java</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J10" s="6" t="str">
         <f t="shared" ref="J10:J15" si="1">"entities["&amp;C10&amp;"]"</f>
         <v>entities[1]</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L10" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C6&amp;"'])"</f>
@@ -8718,7 +8718,7 @@
         <v>212</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F11" s="9" t="str">
         <f>"./generated/"&amp;Entities!G7&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M7,".","/")</f>
@@ -8729,14 +8729,14 @@
         <v>OrderDao.java</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>entities[2]</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L11" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C7&amp;"'])"</f>
@@ -8756,7 +8756,7 @@
         <v>212</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F12" s="9" t="str">
         <f>"./generated/"&amp;Entities!G8&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M8,".","/")</f>
@@ -8767,14 +8767,14 @@
         <v>OrderDetailDao.java</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>entities[3]</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L12" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C8&amp;"'])"</f>
@@ -8794,7 +8794,7 @@
         <v>212</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F13" s="9" t="str">
         <f>"./generated/"&amp;Entities!G9&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M9,".","/")</f>
@@ -8805,14 +8805,14 @@
         <v>ProductDao.java</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>entities[4]</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L13" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C9&amp;"'])"</f>
@@ -8832,7 +8832,7 @@
         <v>212</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F14" s="9" t="str">
         <f>"./generated/"&amp;Entities!G10&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M10,".","/")</f>
@@ -8843,14 +8843,14 @@
         <v>StockDao.java</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>entities[5]</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L14" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C10&amp;"'])"</f>
@@ -8870,7 +8870,7 @@
         <v>212</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F15" s="9" t="str">
         <f>"./generated/"&amp;Entities!G11&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M11,".","/")</f>
@@ -8881,14 +8881,14 @@
         <v>AddressMasterDao.java</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="1"/>
         <v>entities[6]</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L15" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C11&amp;"'])"</f>
@@ -8908,7 +8908,7 @@
         <v>212</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F16" s="9" t="str">
         <f>"./generated/"&amp;Entities!G12&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M12,".","/")</f>
@@ -8919,14 +8919,14 @@
         <v>.java</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" ref="J16:J19" si="3">"entities["&amp;C16&amp;"]"</f>
         <v>entities[7]</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L16" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C12&amp;"'])"</f>
@@ -8946,7 +8946,7 @@
         <v>212</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F17" s="9" t="str">
         <f>"./generated/"&amp;Entities!G13&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M13,".","/")</f>
@@ -8957,14 +8957,14 @@
         <v>.java</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J17" s="6" t="str">
         <f t="shared" si="3"/>
         <v>entities[8]</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L17" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C13&amp;"'])"</f>
@@ -8984,7 +8984,7 @@
         <v>212</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F18" s="9" t="str">
         <f>"./generated/"&amp;Entities!G14&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M14,".","/")</f>
@@ -8995,14 +8995,14 @@
         <v>.java</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J18" s="6" t="str">
         <f t="shared" si="3"/>
         <v>entities[9]</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L18" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C14&amp;"'])"</f>
@@ -9022,7 +9022,7 @@
         <v>212</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F19" s="9" t="str">
         <f>"./generated/"&amp;Entities!G15&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!M15,".","/")</f>
@@ -9033,14 +9033,14 @@
         <v>.java</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J19" s="6" t="str">
         <f t="shared" si="3"/>
         <v>entities[10]</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L19" s="6" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C15&amp;"'])"</f>
@@ -9090,46 +9090,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>257</v>
-      </c>
       <c r="I1" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>288</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -9150,7 +9150,7 @@
     </row>
     <row r="5" spans="1:16" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="21"/>
@@ -9170,7 +9170,7 @@
     </row>
     <row r="8" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>207</v>
@@ -9190,7 +9190,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="14" t="b">
         <f>LEN(G9)&gt;5</f>
@@ -9203,7 +9203,7 @@
         <v>212</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F9" s="14" t="str">
         <f>"./generated/"&amp;Entities!G5&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P5,".","/")</f>
@@ -9214,14 +9214,14 @@
         <v>CustomerMapper.java</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J9" s="14" t="str">
         <f>"entities["&amp;C9&amp;"]"</f>
         <v>entities[0]</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L9" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C5&amp;"'])"</f>
@@ -9245,7 +9245,7 @@
         <v>212</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F10" s="14" t="str">
         <f>"./generated/"&amp;Entities!G6&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P6,".","/")</f>
@@ -9256,14 +9256,14 @@
         <v>CartMapper.java</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J10" s="14" t="str">
         <f t="shared" ref="J10:J19" si="1">"entities["&amp;C10&amp;"]"</f>
         <v>entities[1]</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L10" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C6&amp;"'])"</f>
@@ -9283,7 +9283,7 @@
         <v>212</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F11" s="14" t="str">
         <f>"./generated/"&amp;Entities!G7&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P7,".","/")</f>
@@ -9294,14 +9294,14 @@
         <v>OrderMapper.java</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J11" s="14" t="str">
         <f t="shared" si="1"/>
         <v>entities[2]</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L11" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C7&amp;"'])"</f>
@@ -9321,7 +9321,7 @@
         <v>212</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F12" s="14" t="str">
         <f>"./generated/"&amp;Entities!G8&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P8,".","/")</f>
@@ -9332,14 +9332,14 @@
         <v>OrderDetailMapper.java</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J12" s="14" t="str">
         <f t="shared" si="1"/>
         <v>entities[3]</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L12" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C8&amp;"'])"</f>
@@ -9359,7 +9359,7 @@
         <v>212</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F13" s="14" t="str">
         <f>"./generated/"&amp;Entities!G9&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P9,".","/")</f>
@@ -9370,14 +9370,14 @@
         <v>ProductMapper.java</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J13" s="14" t="str">
         <f t="shared" si="1"/>
         <v>entities[4]</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L13" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C9&amp;"'])"</f>
@@ -9397,7 +9397,7 @@
         <v>212</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F14" s="14" t="str">
         <f>"./generated/"&amp;Entities!G10&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P10,".","/")</f>
@@ -9408,14 +9408,14 @@
         <v>StockMapper.java</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J14" s="14" t="str">
         <f t="shared" si="1"/>
         <v>entities[5]</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L14" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C10&amp;"'])"</f>
@@ -9435,7 +9435,7 @@
         <v>212</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F15" s="14" t="str">
         <f>"./generated/"&amp;Entities!G11&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P11,".","/")</f>
@@ -9446,14 +9446,14 @@
         <v>AddressMasterMapper.java</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J15" s="14" t="str">
         <f t="shared" si="1"/>
         <v>entities[6]</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L15" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C11&amp;"'])"</f>
@@ -9473,7 +9473,7 @@
         <v>212</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F16" s="14" t="str">
         <f>"./generated/"&amp;Entities!G12&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P12,".","/")</f>
@@ -9484,14 +9484,14 @@
         <v>.java</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J16" s="14" t="str">
         <f t="shared" si="1"/>
         <v>entities[7]</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L16" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C12&amp;"'])"</f>
@@ -9511,7 +9511,7 @@
         <v>212</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F17" s="14" t="str">
         <f>"./generated/"&amp;Entities!G13&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P13,".","/")</f>
@@ -9522,14 +9522,14 @@
         <v>.java</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J17" s="14" t="str">
         <f t="shared" si="1"/>
         <v>entities[8]</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L17" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C13&amp;"'])"</f>
@@ -9549,7 +9549,7 @@
         <v>212</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F18" s="14" t="str">
         <f>"./generated/"&amp;Entities!G14&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P14,".","/")</f>
@@ -9560,14 +9560,14 @@
         <v>.java</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J18" s="14" t="str">
         <f t="shared" si="1"/>
         <v>entities[9]</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L18" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C14&amp;"'])"</f>
@@ -9587,7 +9587,7 @@
         <v>212</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F19" s="14" t="str">
         <f>"./generated/"&amp;Entities!G15&amp;"/src/main/java/"&amp;SUBSTITUTE(Entities!P15,".","/")</f>
@@ -9598,14 +9598,14 @@
         <v>.java</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J19" s="14" t="str">
         <f t="shared" si="1"/>
         <v>entities[10]</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L19" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C15&amp;"'])"</f>

</xml_diff>

<commit_message>
Added mapper xml for mapper interface
</commit_message>
<xml_diff>
--- a/AppDefinition.xlsx
+++ b/AppDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="14" r:id="rId1"/>
@@ -21,15 +21,16 @@
     <sheet name="gen_Entity" sheetId="17" r:id="rId7"/>
     <sheet name="gen_DAO" sheetId="19" r:id="rId8"/>
     <sheet name="gen_Mapper" sheetId="23" r:id="rId9"/>
-    <sheet name="gen_MapperGen" sheetId="20" r:id="rId10"/>
-    <sheet name="gen_MapperXmlGen" sheetId="21" r:id="rId11"/>
-    <sheet name="vlookup" sheetId="15" r:id="rId12"/>
-    <sheet name="bk" sheetId="18" r:id="rId13"/>
-    <sheet name="Database-Entity" sheetId="10" r:id="rId14"/>
-    <sheet name="Entity-DB" sheetId="13" r:id="rId15"/>
+    <sheet name="gen_MapperXml" sheetId="25" r:id="rId10"/>
+    <sheet name="gen_MapperGen" sheetId="20" r:id="rId11"/>
+    <sheet name="gen_MapperXmlGen" sheetId="21" r:id="rId12"/>
+    <sheet name="vlookup" sheetId="15" r:id="rId13"/>
+    <sheet name="bk" sheetId="18" r:id="rId14"/>
+    <sheet name="Database-Entity" sheetId="10" r:id="rId15"/>
+    <sheet name="Entity-DB" sheetId="13" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Database-Entity'!$D$3:$D$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'Database-Entity'!$D$3:$D$35</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="318">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -1226,6 +1227,10 @@
   </si>
   <si>
     <t>ddl_h2.txt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mapper_xml.txt</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1291,7 +1296,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1345,6 +1350,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
@@ -1674,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -2315,6 +2326,567 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624FC99C-44CF-4B52-B620-3EA6B5E86366}">
+  <dimension ref="A1:P19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="2" width="10.75" style="20" customWidth="1"/>
+    <col min="3" max="3" width="10.4140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="22.75" style="20" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="104.08203125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.75" style="20"/>
+    <col min="9" max="9" width="9.75" style="20" customWidth="1"/>
+    <col min="10" max="10" width="20.75" style="20" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="44.25" style="20" customWidth="1"/>
+    <col min="13" max="13" width="9.75" style="20" customWidth="1"/>
+    <col min="14" max="14" width="20.75" style="20" customWidth="1"/>
+    <col min="15" max="15" width="9.75" style="20" customWidth="1"/>
+    <col min="16" max="16" width="11.4140625" style="20" customWidth="1"/>
+    <col min="17" max="16384" width="8.75" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="121.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" s="20" t="b">
+        <f>LEN(G9)&gt;5</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F9" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G5&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P5,".","/")</f>
+        <v>./generated/webshop/src/main/resources/org/xlbean/sample/webshop/dao/mapper</v>
+      </c>
+      <c r="G9" s="20" t="str">
+        <f>Entities!Q5&amp;".xml"</f>
+        <v>CustomerMapper.xml</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J9" s="20" t="str">
+        <f>"entities["&amp;C9&amp;"]"</f>
+        <v>entities[0]</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L9" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C5&amp;"'])"</f>
+        <v>properties.findAll(['entityName':'Customer'])</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="20" t="b">
+        <f t="shared" ref="B10:B19" si="0">LEN(G10)&gt;5</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="20">
+        <f>C9+1</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G6&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P6,".","/")</f>
+        <v>./generated/webshop/src/main/resources/org/xlbean/sample/webshop/dao/mapper</v>
+      </c>
+      <c r="G10" s="20" t="str">
+        <f>Entities!Q6&amp;".xml"</f>
+        <v>CartMapper.xml</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J10" s="20" t="str">
+        <f t="shared" ref="J10:J19" si="1">"entities["&amp;C10&amp;"]"</f>
+        <v>entities[1]</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L10" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C6&amp;"'])"</f>
+        <v>properties.findAll(['entityName':'Cart'])</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11" s="20">
+        <f t="shared" ref="C11:C19" si="2">C10+1</f>
+        <v>2</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F11" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G7&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P7,".","/")</f>
+        <v>./generated/webshop/src/main/resources/org/xlbean/sample/webshop/dao/mapper</v>
+      </c>
+      <c r="G11" s="20" t="str">
+        <f>Entities!Q7&amp;".xml"</f>
+        <v>OrderMapper.xml</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J11" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>entities[2]</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L11" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C7&amp;"'])"</f>
+        <v>properties.findAll(['entityName':'Order'])</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C12" s="20">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F12" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G8&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P8,".","/")</f>
+        <v>./generated/webshop/src/main/resources/org/xlbean/sample/webshop/dao/mapper</v>
+      </c>
+      <c r="G12" s="20" t="str">
+        <f>Entities!Q8&amp;".xml"</f>
+        <v>OrderDetailMapper.xml</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>entities[3]</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L12" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C8&amp;"'])"</f>
+        <v>properties.findAll(['entityName':'OrderDetail'])</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C13" s="20">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F13" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G9&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P9,".","/")</f>
+        <v>./generated/webshop/src/main/resources/org/xlbean/sample/webshop/dao/mapper</v>
+      </c>
+      <c r="G13" s="20" t="str">
+        <f>Entities!Q9&amp;".xml"</f>
+        <v>ProductMapper.xml</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J13" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>entities[4]</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L13" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C9&amp;"'])"</f>
+        <v>properties.findAll(['entityName':'Product'])</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C14" s="20">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F14" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G10&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P10,".","/")</f>
+        <v>./generated/webshop/src/main/resources/org/xlbean/sample/webshop/dao/mapper</v>
+      </c>
+      <c r="G14" s="20" t="str">
+        <f>Entities!Q10&amp;".xml"</f>
+        <v>StockMapper.xml</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J14" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>entities[5]</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L14" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C10&amp;"'])"</f>
+        <v>properties.findAll(['entityName':'Stock'])</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C15" s="20">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F15" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G11&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P11,".","/")</f>
+        <v>./generated/webshop/src/main/resources/org/xlbean/sample/webshop/dao/mapper</v>
+      </c>
+      <c r="G15" s="20" t="str">
+        <f>Entities!Q11&amp;".xml"</f>
+        <v>AddressMasterMapper.xml</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J15" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>entities[6]</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L15" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C11&amp;"'])"</f>
+        <v>properties.findAll(['entityName':'AddressMaster'])</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C16" s="20">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F16" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G12&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P12,".","/")</f>
+        <v>./generated//src/main/resources/</v>
+      </c>
+      <c r="G16" s="20" t="str">
+        <f>Entities!Q12&amp;".xml"</f>
+        <v>.xml</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J16" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>entities[7]</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L16" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C12&amp;"'])"</f>
+        <v>properties.findAll(['entityName':''])</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C17" s="20">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F17" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G13&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P13,".","/")</f>
+        <v>./generated//src/main/resources/</v>
+      </c>
+      <c r="G17" s="20" t="str">
+        <f>Entities!Q13&amp;".xml"</f>
+        <v>.xml</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J17" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>entities[8]</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L17" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C13&amp;"'])"</f>
+        <v>properties.findAll(['entityName':''])</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C18" s="20">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F18" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G14&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P14,".","/")</f>
+        <v>./generated//src/main/resources/</v>
+      </c>
+      <c r="G18" s="20" t="str">
+        <f>Entities!Q14&amp;".xml"</f>
+        <v>.xml</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J18" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>entities[9]</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L18" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C14&amp;"'])"</f>
+        <v>properties.findAll(['entityName':''])</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C19" s="20">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="F19" s="20" t="str">
+        <f>"./generated/"&amp;Entities!G15&amp;"/src/main/resources/"&amp;SUBSTITUTE(Entities!P15,".","/")</f>
+        <v>./generated//src/main/resources/</v>
+      </c>
+      <c r="G19" s="20" t="str">
+        <f>Entities!Q15&amp;".xml"</f>
+        <v>.xml</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J19" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>entities[10]</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L19" s="20" t="str">
+        <f>"properties.findAll(['entityName':'"&amp;Entities!C15&amp;"'])"</f>
+        <v>properties.findAll(['entityName':''])</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:J5"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
@@ -2409,15 +2981,15 @@
       <c r="A5" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="8"/>
@@ -2879,7 +3451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
@@ -2974,15 +3546,15 @@
       <c r="A5" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="8"/>
@@ -3444,7 +4016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -3514,7 +4086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3527,7 +4099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:S35"/>
   <sheetViews>
@@ -4649,7 +5221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="B1:R31"/>
   <sheetViews>
@@ -7196,7 +7768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:J5"/>
     </sheetView>
   </sheetViews>
@@ -7286,17 +7858,17 @@
       <c r="A5" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>312</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="2"/>
@@ -7453,15 +8025,15 @@
       <c r="A5" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="15"/>
@@ -8018,15 +8590,15 @@
       <c r="A5" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="3"/>
@@ -8587,15 +9159,15 @@
       <c r="A5" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="5"/>
@@ -9061,9 +9633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:J5"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -9152,15 +9722,15 @@
       <c r="A5" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="13"/>
@@ -9226,10 +9796,6 @@
       <c r="L9" s="14" t="str">
         <f>"properties.findAll(['entityName':'"&amp;Entities!C5&amp;"'])"</f>
         <v>properties.findAll(['entityName':'Customer'])</v>
-      </c>
-      <c r="P9" s="14">
-        <f>C9</f>
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">

</xml_diff>